<commit_message>
Add solution task 1 for pairwise testing
</commit_message>
<xml_diff>
--- a/Pairwise testing/Задание 1.xlsx
+++ b/Pairwise testing/Задание 1.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Task1" sheetId="1" r:id="rId1"/>
+    <sheet name="Pairwise" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="17">
   <si>
     <t>Шрифт</t>
   </si>
@@ -67,13 +68,16 @@
   </si>
   <si>
     <t>Начертание</t>
+  </si>
+  <si>
+    <t>OC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,6 +91,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -127,16 +142,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -416,7 +439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -494,4 +517,362 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4">
+        <v>16</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4">
+        <v>14</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="4">
+        <v>14</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="4">
+        <v>16</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="4">
+        <v>14</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4">
+        <v>14</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="4">
+        <v>16</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="4">
+        <v>14</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="4">
+        <v>14</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="4">
+        <v>14</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="4">
+        <v>16</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="4">
+        <v>14</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="4">
+        <v>16</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add All Combinations of pairwise testing for task 1
</commit_message>
<xml_diff>
--- a/Pairwise testing/Задание 1.xlsx
+++ b/Pairwise testing/Задание 1.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Task1" sheetId="1" r:id="rId1"/>
     <sheet name="Pairwise" sheetId="2" r:id="rId2"/>
+    <sheet name="AllCombinations" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="17">
   <si>
     <t>Шрифт</t>
   </si>
@@ -146,7 +147,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -154,6 +155,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -523,7 +530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -875,4 +882,1512 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="5">
+        <v>14</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5">
+        <v>14</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5">
+        <v>14</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="5">
+        <v>14</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="5">
+        <v>14</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="5">
+        <v>14</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="5">
+        <v>14</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="5">
+        <v>14</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="5">
+        <v>14</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="5">
+        <v>14</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="5">
+        <v>14</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="5">
+        <v>14</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="5">
+        <v>14</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="5">
+        <v>14</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="5">
+        <v>14</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="5">
+        <v>14</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="5">
+        <v>16</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="5">
+        <v>16</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="5">
+        <v>16</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="5">
+        <v>16</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="5">
+        <v>16</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>22</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="5">
+        <v>16</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>23</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="5">
+        <v>16</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
+        <v>24</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="5">
+        <v>16</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>25</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="5">
+        <v>16</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <v>26</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="5">
+        <v>16</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>27</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="5">
+        <v>16</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
+        <v>28</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="5">
+        <v>16</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
+        <v>29</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="5">
+        <v>16</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
+        <v>30</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="5">
+        <v>16</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
+        <v>31</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="5">
+        <v>16</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
+        <v>32</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="5">
+        <v>16</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
+        <v>33</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="5">
+        <v>14</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="6">
+        <v>34</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="5">
+        <v>14</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="6">
+        <v>35</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="5">
+        <v>14</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="6">
+        <v>36</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="5">
+        <v>14</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="6">
+        <v>37</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="5">
+        <v>14</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="6">
+        <v>38</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="5">
+        <v>14</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="6">
+        <v>39</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="5">
+        <v>14</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="6">
+        <v>40</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="5">
+        <v>14</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="6">
+        <v>41</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" s="5">
+        <v>14</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="6">
+        <v>42</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" s="5">
+        <v>14</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="6">
+        <v>43</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" s="5">
+        <v>14</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="6">
+        <v>44</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="5">
+        <v>14</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="6">
+        <v>45</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" s="5">
+        <v>14</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="6">
+        <v>46</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" s="5">
+        <v>14</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="6">
+        <v>47</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" s="5">
+        <v>14</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="6">
+        <v>48</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" s="5">
+        <v>14</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="6">
+        <v>49</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" s="5">
+        <v>16</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="6">
+        <v>50</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" s="5">
+        <v>16</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="6">
+        <v>51</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" s="5">
+        <v>16</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="6">
+        <v>52</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" s="5">
+        <v>16</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="6">
+        <v>53</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C54" s="5">
+        <v>16</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="6">
+        <v>54</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" s="5">
+        <v>16</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="6">
+        <v>55</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56" s="5">
+        <v>16</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="6">
+        <v>56</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57" s="5">
+        <v>16</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="6">
+        <v>57</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C58" s="5">
+        <v>16</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="6">
+        <v>58</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59" s="5">
+        <v>16</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="6">
+        <v>59</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" s="5">
+        <v>16</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="6">
+        <v>60</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" s="5">
+        <v>16</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="6">
+        <v>61</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C62" s="5">
+        <v>16</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="6">
+        <v>62</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C63" s="5">
+        <v>16</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="6">
+        <v>63</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C64" s="5">
+        <v>16</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="6">
+        <v>64</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C65" s="5">
+        <v>16</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>